<commit_message>
Added appShellFiles constant to the serviceworker.js file
</commit_message>
<xml_diff>
--- a/paying participants.xlsx
+++ b/paying participants.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Nb</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>Amount left to reimburse</t>
+  </si>
+  <si>
+    <t>Bobo Benda Ulrich Gregore</t>
   </si>
 </sst>
 </file>
@@ -360,10 +363,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -416,6 +419,27 @@
         <v>200</v>
       </c>
     </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>699003156</v>
+      </c>
+      <c r="D3">
+        <v>500</v>
+      </c>
+      <c r="E3">
+        <v>200</v>
+      </c>
+      <c r="F3">
+        <f>D3-E3-300</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Registered 2 new players
</commit_message>
<xml_diff>
--- a/paying participants.xlsx
+++ b/paying participants.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Nb</t>
   </si>
@@ -46,6 +46,12 @@
   </si>
   <si>
     <t>Bobo Benda Ulrich Gregore</t>
+  </si>
+  <si>
+    <t>SIKATI KENMOGNE Samuel</t>
+  </si>
+  <si>
+    <t>Motso Daniel Kevin</t>
   </si>
 </sst>
 </file>
@@ -363,10 +369,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -440,6 +446,47 @@
         <v>0</v>
       </c>
     </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4">
+        <v>657407989</v>
+      </c>
+      <c r="D4">
+        <v>500</v>
+      </c>
+      <c r="E4">
+        <v>200</v>
+      </c>
+      <c r="F4">
+        <f>D4-E4-300</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>693851447</v>
+      </c>
+      <c r="D5">
+        <v>350</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Songsare Pierre to the excel file
</commit_message>
<xml_diff>
--- a/paying participants.xlsx
+++ b/paying participants.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>Nb</t>
   </si>
@@ -52,6 +52,18 @@
   </si>
   <si>
     <t>Motso Daniel Kevin</t>
+  </si>
+  <si>
+    <t>Method</t>
+  </si>
+  <si>
+    <t>cash</t>
+  </si>
+  <si>
+    <t>momo</t>
+  </si>
+  <si>
+    <t>Songsare Amdji Pierre</t>
   </si>
 </sst>
 </file>
@@ -369,10 +381,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -380,11 +392,12 @@
     <col min="2" max="2" width="27.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -398,13 +411,16 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -417,15 +433,18 @@
       <c r="D2">
         <v>500</v>
       </c>
-      <c r="E2">
-        <v>0</v>
+      <c r="E2" t="s">
+        <v>12</v>
       </c>
       <c r="F2">
-        <f>D2-E2-300</f>
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <f>D2-F2-300</f>
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -438,15 +457,18 @@
       <c r="D3">
         <v>500</v>
       </c>
-      <c r="E3">
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3">
         <v>200</v>
       </c>
-      <c r="F3">
-        <f>D3-E3-300</f>
+      <c r="G3">
+        <f>D3-F3-300</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -459,15 +481,18 @@
       <c r="D4">
         <v>500</v>
       </c>
-      <c r="E4">
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4">
         <v>200</v>
       </c>
-      <c r="F4">
-        <f>D4-E4-300</f>
+      <c r="G4">
+        <f t="shared" ref="G4:G6" si="0">D4-F4-300</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -480,10 +505,38 @@
       <c r="D5">
         <v>350</v>
       </c>
-      <c r="E5">
-        <v>0</v>
+      <c r="E5" t="s">
+        <v>13</v>
       </c>
       <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6">
+        <v>694865719</v>
+      </c>
+      <c r="D6">
+        <v>300</v>
+      </c>
+      <c r="E6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Made login and signup visible on mobile
</commit_message>
<xml_diff>
--- a/paying participants.xlsx
+++ b/paying participants.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
   <si>
     <t>Nb</t>
   </si>
@@ -67,6 +67,30 @@
   </si>
   <si>
     <t>NJEMBE MATHIEU</t>
+  </si>
+  <si>
+    <t>Tchomb Joseph Loic</t>
+  </si>
+  <si>
+    <t>Bayeck Joseph</t>
+  </si>
+  <si>
+    <t>695919585, 675366970</t>
+  </si>
+  <si>
+    <t>Mabou Fotso Kevin</t>
+  </si>
+  <si>
+    <t>Rikam Yvanol</t>
+  </si>
+  <si>
+    <t>Mbame Mbame Martin</t>
+  </si>
+  <si>
+    <t>Noua Aimerick</t>
+  </si>
+  <si>
+    <t>Hans Manfred ngalle</t>
   </si>
 </sst>
 </file>
@@ -384,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,8 +539,7 @@
         <v>0</v>
       </c>
       <c r="G5">
-        <f t="shared" si="0"/>
-        <v>50</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -567,7 +590,169 @@
         <v>0</v>
       </c>
     </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8">
+        <v>657489972</v>
+      </c>
+      <c r="D8">
+        <v>350</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9">
+        <v>500</v>
+      </c>
+      <c r="E9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9">
+        <v>200</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10">
+        <v>657936031</v>
+      </c>
+      <c r="D10">
+        <v>500</v>
+      </c>
+      <c r="E10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10">
+        <v>200</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11">
+        <v>6553722422</v>
+      </c>
+      <c r="D11">
+        <v>300</v>
+      </c>
+      <c r="E11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12">
+        <v>697720509</v>
+      </c>
+      <c r="D12">
+        <v>300</v>
+      </c>
+      <c r="E12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13">
+        <v>674743317</v>
+      </c>
+      <c r="D13">
+        <v>300</v>
+      </c>
+      <c r="E13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14">
+        <v>650469243</v>
+      </c>
+      <c r="D14">
+        <v>1000</v>
+      </c>
+      <c r="E14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14">
+        <v>700</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added an endpoint for checking unique values instead of returing them from a GET request
</commit_message>
<xml_diff>
--- a/paying participants.xlsx
+++ b/paying participants.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
   <si>
     <t>Nb</t>
   </si>
@@ -91,6 +91,12 @@
   </si>
   <si>
     <t>Hans Manfred ngalle</t>
+  </si>
+  <si>
+    <t>Tsembom Percy</t>
+  </si>
+  <si>
+    <t>Tchielong Gaius</t>
   </si>
 </sst>
 </file>
@@ -408,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -491,7 +497,7 @@
         <v>200</v>
       </c>
       <c r="G3">
-        <f>D3-F3-300</f>
+        <f t="shared" ref="G3:G16" si="0">D3-F3-300</f>
         <v>0</v>
       </c>
     </row>
@@ -515,7 +521,7 @@
         <v>200</v>
       </c>
       <c r="G4">
-        <f t="shared" ref="G4:G7" si="0">D4-F4-300</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -539,7 +545,8 @@
         <v>0</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -610,7 +617,8 @@
         <v>0</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -633,6 +641,7 @@
         <v>200</v>
       </c>
       <c r="G9">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -656,6 +665,7 @@
         <v>200</v>
       </c>
       <c r="G10">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -679,6 +689,7 @@
         <v>0</v>
       </c>
       <c r="G11">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -702,6 +713,7 @@
         <v>0</v>
       </c>
       <c r="G12">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -725,6 +737,7 @@
         <v>0</v>
       </c>
       <c r="G13">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -748,7 +761,56 @@
         <v>700</v>
       </c>
       <c r="G14">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15">
+        <v>692201677</v>
+      </c>
+      <c r="D15">
+        <v>300</v>
+      </c>
+      <c r="E15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16">
+        <v>695044180</v>
+      </c>
+      <c r="D16">
+        <v>1000</v>
+      </c>
+      <c r="E16" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16">
+        <v>500</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Displaying terms and conditions in popup when player chooses to enroll
</commit_message>
<xml_diff>
--- a/paying participants.xlsx
+++ b/paying participants.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="30">
   <si>
     <t>Nb</t>
   </si>
@@ -97,6 +97,18 @@
   </si>
   <si>
     <t>Tchielong Gaius</t>
+  </si>
+  <si>
+    <t>Ndjiki</t>
+  </si>
+  <si>
+    <t>Dasse</t>
+  </si>
+  <si>
+    <t>Gaetan Aymar</t>
+  </si>
+  <si>
+    <t>Amombo Ngongo</t>
   </si>
 </sst>
 </file>
@@ -414,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -497,7 +509,7 @@
         <v>200</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G16" si="0">D3-F3-300</f>
+        <f t="shared" ref="G3:G19" si="0">D3-F3-300</f>
         <v>0</v>
       </c>
     </row>
@@ -810,6 +822,98 @@
       </c>
       <c r="G16">
         <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17">
+        <v>690839895</v>
+      </c>
+      <c r="D17">
+        <v>300</v>
+      </c>
+      <c r="E17" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18">
+        <v>694993298</v>
+      </c>
+      <c r="D18">
+        <v>300</v>
+      </c>
+      <c r="E18" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19">
+        <v>691674935</v>
+      </c>
+      <c r="D19">
+        <v>500</v>
+      </c>
+      <c r="E19" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19">
+        <v>100</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20">
+        <v>691569975</v>
+      </c>
+      <c r="D20">
+        <v>500</v>
+      </c>
+      <c r="E20" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20">
         <v>200</v>
       </c>
     </row>

</xml_diff>